<commit_message>
more pick and place preparation
</commit_message>
<xml_diff>
--- a/rev_b/hdw/Pulse_Oximeter/pick_and_place/feeders_data_sample.xlsx
+++ b/rev_b/hdw/Pulse_Oximeter/pick_and_place/feeders_data_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\pulse_oximeter\rev_b\hdw\Pulse_Oximeter\pick_and_place\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C015A5C-D6C5-4BAB-89F0-ACF47A3E6744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5830F814-96B4-4F57-8D15-214686536305}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="44">
   <si>
     <t>Tape Size</t>
   </si>
@@ -123,19 +123,10 @@
     <t>10uF-C_0402</t>
   </si>
   <si>
-    <t>10-R_0402</t>
-  </si>
-  <si>
     <t>10nF-C_0402</t>
   </si>
   <si>
-    <t>1nF-C_0402</t>
-  </si>
-  <si>
     <t>1k-R_0402</t>
-  </si>
-  <si>
-    <t>74LVC1G06-SOT-353_SC-70-5</t>
   </si>
   <si>
     <t>Green-LED_0402</t>
@@ -145,6 +136,27 @@
   </si>
   <si>
     <t>PIC32MZ0512EFE064T-I_PT-TQFP-64_10x10mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>0-R_0402</t>
+  </si>
+  <si>
+    <t>600R_0.5A-L_0402</t>
+  </si>
+  <si>
+    <t>100-R_0402</t>
+  </si>
+  <si>
+    <t>100k-R_0402</t>
+  </si>
+  <si>
+    <t>10uF-C_1206</t>
+  </si>
+  <si>
+    <t>74LVC1G97-SOT-363_SC-70-6</t>
+  </si>
+  <si>
+    <t>BSS214NW-SOT-323_SC-70</t>
   </si>
 </sst>
 </file>
@@ -189,7 +201,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -562,7 +573,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1092,19 +1103,19 @@
       <c r="E11" s="3">
         <v>0</v>
       </c>
-      <c r="F11" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="F11" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9">
         <v>2</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="9">
         <v>90</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="9">
         <v>2</v>
       </c>
       <c r="K11" s="3" t="s">
@@ -1132,8 +1143,8 @@
       <c r="B12" s="3">
         <v>11</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>32</v>
+      <c r="C12" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -1182,7 +1193,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -1230,28 +1241,28 @@
       <c r="B14" s="3">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
+      <c r="C14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="9">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0</v>
+      </c>
+      <c r="F14" s="9">
         <v>0.5</v>
       </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="G14" s="9">
+        <v>0</v>
+      </c>
+      <c r="H14" s="9">
         <v>2</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="9">
         <v>90</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="9">
         <v>2</v>
       </c>
       <c r="K14" s="3" t="s">
@@ -1280,7 +1291,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D15" s="3">
         <v>0</v>
@@ -1328,8 +1339,8 @@
       <c r="B16" s="3">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>36</v>
+      <c r="C16" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
@@ -1337,7 +1348,7 @@
       <c r="E16" s="3">
         <v>0</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="9">
         <v>1</v>
       </c>
       <c r="G16" s="3">
@@ -1349,7 +1360,9 @@
       <c r="I16" s="9">
         <v>90</v>
       </c>
-      <c r="J16" s="3"/>
+      <c r="J16" s="9">
+        <v>4</v>
+      </c>
       <c r="K16" s="3" t="s">
         <v>19</v>
       </c>
@@ -1376,7 +1389,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
@@ -1396,7 +1409,7 @@
       <c r="I17" s="9">
         <v>90</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="9">
         <v>4</v>
       </c>
       <c r="K17" s="3" t="s">
@@ -1425,7 +1438,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3">
         <v>0</v>
@@ -1445,7 +1458,7 @@
       <c r="I18" s="9">
         <v>90</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="9">
         <v>4</v>
       </c>
       <c r="K18" s="3" t="s">
@@ -1473,8 +1486,8 @@
       <c r="B19" s="3">
         <v>18</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>18</v>
+      <c r="C19" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="D19" s="3">
         <v>0</v>
@@ -1483,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
@@ -1495,7 +1508,7 @@
         <v>90</v>
       </c>
       <c r="J19" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>19</v>
@@ -1522,8 +1535,8 @@
       <c r="B20" s="3">
         <v>19</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>18</v>
+      <c r="C20" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="D20" s="3">
         <v>0</v>
@@ -1532,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
@@ -1544,7 +1557,7 @@
         <v>90</v>
       </c>
       <c r="J20" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>19</v>
@@ -1571,28 +1584,28 @@
       <c r="B21" s="3">
         <v>20</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="3">
-        <v>0</v>
-      </c>
-      <c r="E21" s="3">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G21" s="3">
-        <v>0</v>
-      </c>
-      <c r="H21" s="3">
+      <c r="C21" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9">
+        <v>1.8</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
         <v>2</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="9">
         <v>90</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="9">
         <v>4</v>
       </c>
       <c r="K21" s="3" t="s">
@@ -1620,28 +1633,28 @@
       <c r="B22" s="3">
         <v>21</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G22" s="3">
-        <v>0</v>
-      </c>
-      <c r="H22" s="3">
+      <c r="C22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
         <v>2</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="9">
         <v>90</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="9">
         <v>4</v>
       </c>
       <c r="K22" s="3" t="s">
@@ -2021,7 +2034,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D30" s="3">
         <v>0</v>
@@ -2038,8 +2051,12 @@
       <c r="H30" s="3">
         <v>1</v>
       </c>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="3">
+        <v>-90</v>
+      </c>
+      <c r="J30" s="3">
+        <v>12</v>
+      </c>
       <c r="K30" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
added rev b doc
</commit_message>
<xml_diff>
--- a/rev_b/hdw/Pulse_Oximeter/pick_and_place/feeders_data_sample.xlsx
+++ b/rev_b/hdw/Pulse_Oximeter/pick_and_place/feeders_data_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Drew Maatman\Documents\KiCad Projects\Projects\pulse_oximeter\rev_b\hdw\Pulse_Oximeter\pick_and_place\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5830F814-96B4-4F57-8D15-214686536305}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D678EF25-BDC3-4D27-BD95-21C1F35A916E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="54">
   <si>
     <t>Tape Size</t>
   </si>
@@ -158,6 +158,36 @@
   <si>
     <t>BSS214NW-SOT-323_SC-70</t>
   </si>
+  <si>
+    <t>Trays:</t>
+  </si>
+  <si>
+    <t>100uF Tantalum</t>
+  </si>
+  <si>
+    <t>3.3uH</t>
+  </si>
+  <si>
+    <t>TPS26600</t>
+  </si>
+  <si>
+    <t>TPS62152</t>
+  </si>
+  <si>
+    <t>TPS7A7200</t>
+  </si>
+  <si>
+    <t>TXB0102</t>
+  </si>
+  <si>
+    <t>TPS22929</t>
+  </si>
+  <si>
+    <t>MAX30102</t>
+  </si>
+  <si>
+    <t>AT42Q</t>
+  </si>
 </sst>
 </file>
 
@@ -166,7 +196,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C];[Red]\-#,##0.00\ [$€-40C]"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -204,6 +234,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,7 +272,7 @@
       <alignment textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -253,6 +295,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading1" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -572,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -996,7 +1042,7 @@
       <c r="B9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="3">
@@ -1045,7 +1091,7 @@
       <c r="B10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="3">
@@ -1094,7 +1140,7 @@
       <c r="B11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="3">
@@ -1143,7 +1189,7 @@
       <c r="B12" s="3">
         <v>11</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="3">
@@ -1192,7 +1238,7 @@
       <c r="B13" s="3">
         <v>12</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="10" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="3">
@@ -1241,7 +1287,7 @@
       <c r="B14" s="3">
         <v>13</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="9">
@@ -1290,7 +1336,7 @@
       <c r="B15" s="3">
         <v>14</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D15" s="3">
@@ -1339,7 +1385,7 @@
       <c r="B16" s="3">
         <v>15</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="3">
@@ -1388,7 +1434,7 @@
       <c r="B17" s="3">
         <v>16</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D17" s="3">
@@ -1437,7 +1483,7 @@
       <c r="B18" s="3">
         <v>17</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D18" s="3">
@@ -1486,7 +1532,7 @@
       <c r="B19" s="3">
         <v>18</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="3">
@@ -1535,7 +1581,7 @@
       <c r="B20" s="3">
         <v>19</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="3">
@@ -1584,7 +1630,7 @@
       <c r="B21" s="3">
         <v>20</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="9">
@@ -1633,7 +1679,7 @@
       <c r="B22" s="3">
         <v>21</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="9">
@@ -2236,7 +2282,9 @@
     <row r="37" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="C37" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -2255,10 +2303,14 @@
     <row r="38" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="C38" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="F38" s="3">
+        <v>3.1</v>
+      </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2274,10 +2326,14 @@
     <row r="39" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="F39" s="3">
+        <v>2</v>
+      </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -2293,10 +2349,14 @@
     <row r="40" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="C40" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3">
+        <v>1</v>
+      </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
@@ -2309,16 +2369,33 @@
       <c r="P40" s="3"/>
       <c r="Q40" s="3"/>
     </row>
+    <row r="41" spans="1:17" ht="14" x14ac:dyDescent="0.3">
+      <c r="C41" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="9">
+        <v>1</v>
+      </c>
+    </row>
     <row r="42" spans="1:17" ht="14" x14ac:dyDescent="0.3">
-      <c r="C42" s="2"/>
+      <c r="C42" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
+      <c r="C43" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="F43" s="3">
+        <v>0.8</v>
+      </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
@@ -2334,10 +2411,14 @@
     <row r="44" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="C44" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3">
+        <v>1.4</v>
+      </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
@@ -2353,7 +2434,9 @@
     <row r="45" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="C45" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -2372,7 +2455,9 @@
     <row r="46" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="C46" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>

</xml_diff>